<commit_message>
Update spreadsheet with simulations
</commit_message>
<xml_diff>
--- a/gameSims3.xlsx
+++ b/gameSims3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="gameSims3" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="49">
   <si>
     <t xml:space="preserve">Goblin</t>
   </si>
@@ -165,6 +165,9 @@
   <si>
     <t xml:space="preserve">[20</t>
   </si>
+  <si>
+    <t xml:space="preserve">[-2</t>
+  </si>
 </sst>
 </file>
 
@@ -259,9 +262,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BF65"/>
+  <dimension ref="A1:BF80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5292,6 +5295,924 @@
         <v>3</v>
       </c>
     </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="X66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y66" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA66" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M67" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N67" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O67" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P67" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q67" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S68" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U68" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M69" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O69" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q69" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S69" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K70" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L70" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M70" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N70" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O70" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P70" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q70" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K71" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L71" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N71" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O71" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R71" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S71" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L72" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N72" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O72" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="S72" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T72" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K73" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L73" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N73" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P73" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q73" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L74" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S74" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L75" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M75" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q75" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="T75" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R76" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="S76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V76" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="W76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y76" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L77" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N77" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O77" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="K78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P78" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q78" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="T78" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="U78" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K79" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L79" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M79" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N79" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O79" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P79" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q79" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="K80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="M80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P80" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="S80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T80" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="U80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="V80" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Update excel version of survey data
</commit_message>
<xml_diff>
--- a/gameSims3.xlsx
+++ b/gameSims3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="gameSims3" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="54">
   <si>
     <t xml:space="preserve">Goblin</t>
   </si>
@@ -168,6 +168,21 @@
   <si>
     <t xml:space="preserve">[-2</t>
   </si>
+  <si>
+    <t xml:space="preserve">Beserker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12]</t>
+  </si>
 </sst>
 </file>
 
@@ -262,9 +277,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BF80"/>
+  <dimension ref="A1:BF105"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6213,6 +6228,1460 @@
         <v>6</v>
       </c>
     </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O81" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O82" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q82" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S82" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="V82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="W82" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K83" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M83" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O83" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K84" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M84" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O84" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K85" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M85" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N86" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P86" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q86" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="R86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="U86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="V86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="W86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="X86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y86" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z86" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA86" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB86" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J87" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L87" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M87" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N87" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O87" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P87" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q87" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K88" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M88" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N88" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H89" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I89" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J89" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K89" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L89" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M89" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="N89" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O89" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q89" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R89" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S89" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J90" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K90" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L90" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N90" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O90" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R90" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S90" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T90" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U90" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P91" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q91" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R91" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M92" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O92" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P92" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q92" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E93" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q93" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R93" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="S93" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K94" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O94" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I95" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="J95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O95" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K96" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M96" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="O96" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P96" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q96" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R96" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="L97" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="M97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N97" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P97" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S97" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="T97" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H98" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="I98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K98" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L98" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N98" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P98" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S98" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="T98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U98" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F99" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="H99" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="I99" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J99" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="K99" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L99" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="N99" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="O99" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P99" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J100" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N100" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="P100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="T100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="U100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="V100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W100" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="X100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB100" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC100" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J101" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K101" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L101" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="P101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="R101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S101" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="T101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U101" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W101" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J102" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K102" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L102" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M102" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O102" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q102" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="R102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="S102" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="T102" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="U102" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J103" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K103" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L103" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M103" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="N103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O103" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J104" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K104" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="L104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="M104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N104" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O104" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q104" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="R104" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="S104" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="T104" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U104" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="V104" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="W104" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="X104" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J105" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="K105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L105" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="M105" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="N105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="O105" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="P105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q105" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>